<commit_message>
adds Lawfulness: EU-DGA, EU-AIAct, EU-NIS2; closes #170
- each legal extension has its own Lawfulness concept with enumeration
  Compliance, NonCompliant, and ComplianceUnknown
- terms added in CSV (source), and RDF and HTML
- NIS2 HTML has a notice that the compliance depends on member state
  implementations as it is a directive
</commit_message>
<xml_diff>
--- a/code/vocab_csv/eu-dga.xlsx
+++ b/code/vocab_csv/eu-dga.xlsx
@@ -10,6 +10,7 @@
     <sheet state="visible" name="DGA_TOMs" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="DGA_entities" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="DGA_properties" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="DGA_compliance" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="270">
   <si>
     <t>Term</t>
   </si>
@@ -846,6 +847,54 @@
   </si>
   <si>
     <t>Indicates association with data intermediation service provider</t>
+  </si>
+  <si>
+    <t>DGA specific statuses in dpv-DGA</t>
+  </si>
+  <si>
+    <t>DGALawfulness</t>
+  </si>
+  <si>
+    <t>DGA Lawfulness</t>
+  </si>
+  <si>
+    <t>Status or state associated with being lawful or legally compliant regarding DGA</t>
+  </si>
+  <si>
+    <t>dpv:Lawfulness</t>
+  </si>
+  <si>
+    <t>Harshvardhan J. Pandit, Beatriz Esteves</t>
+  </si>
+  <si>
+    <t>DGACompliant</t>
+  </si>
+  <si>
+    <t>DGA Compliant</t>
+  </si>
+  <si>
+    <t>State of being lawful or legally compliant for DGA</t>
+  </si>
+  <si>
+    <t>eu-dga:DGALawfulness</t>
+  </si>
+  <si>
+    <t>DGANonCompliant</t>
+  </si>
+  <si>
+    <t>DGA Non-compliant</t>
+  </si>
+  <si>
+    <t>State of being unlawful or legally non-compliant for DGA</t>
+  </si>
+  <si>
+    <t>DGAComplianceUnknown</t>
+  </si>
+  <si>
+    <t>DGA Compliance Unknown</t>
+  </si>
+  <si>
+    <t>State where lawfulness or compliance with DGA is unknown</t>
   </si>
 </sst>
 </file>
@@ -1288,6 +1337,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
@@ -11307,4 +11360,704 @@
   </conditionalFormatting>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="32.13"/>
+    <col customWidth="1" min="2" max="2" width="20.88"/>
+    <col customWidth="1" min="3" max="3" width="38.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="28.5" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>257</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="13">
+        <v>45494.0</v>
+      </c>
+      <c r="L3" s="10"/>
+      <c r="M3" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="O3" s="9"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>262</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="13">
+        <v>45494.0</v>
+      </c>
+      <c r="L4" s="10"/>
+      <c r="M4" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="O4" s="9"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="38" t="s">
+        <v>264</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="13">
+        <v>45494.0</v>
+      </c>
+      <c r="L5" s="10"/>
+      <c r="M5" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="O5" s="9"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>269</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="13">
+        <v>45494.0</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="M6" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="O6" s="9"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="16"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="10"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="16"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="10"/>
+      <c r="AE8" s="10"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="16"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="10"/>
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="10"/>
+      <c r="AD9" s="10"/>
+      <c r="AE9" s="10"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="10"/>
+      <c r="AE10" s="10"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10"/>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="10"/>
+      <c r="AE11" s="10"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="40"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="10"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="10"/>
+      <c r="AB13" s="10"/>
+      <c r="AC13" s="10"/>
+      <c r="AD13" s="10"/>
+      <c r="AE13" s="10"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="10"/>
+      <c r="AD14" s="10"/>
+      <c r="AE14" s="10"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="10"/>
+      <c r="AD15" s="10"/>
+      <c r="AE15" s="10"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="10"/>
+      <c r="AC16" s="10"/>
+      <c r="AD16" s="10"/>
+      <c r="AE16" s="10"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="10"/>
+      <c r="AD17" s="10"/>
+      <c r="AE17" s="10"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="10"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="10"/>
+      <c r="AB18" s="10"/>
+      <c r="AC18" s="10"/>
+      <c r="AD18" s="10"/>
+      <c r="AE18" s="10"/>
+    </row>
+    <row r="19">
+      <c r="K19" s="13"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:AE43">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$M2="accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:AE43">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$M2="proposed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:AE43">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$M2="changed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>